<commit_message>
refactor(template excel): cstring to string
</commit_message>
<xml_diff>
--- a/public/template/upload-tag-template.xlsx
+++ b/public/template/upload-tag-template.xlsx
@@ -45,10 +45,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -82,14 +82,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -104,77 +96,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,15 +110,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,6 +141,74 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -225,13 +225,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -243,163 +399,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,6 +441,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -451,6 +466,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -469,188 +510,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -991,7 +991,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="23.2" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1037,8 +1037,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5 C6:C7 C8:C13 C14:C1048576">
       <formula1>"Read,Write,Subscribe,Read Write,Read Subscribe,Write Subscribe,Read Write Subscribe"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13 D14:D1048576">
-      <formula1>"BYTE,INT8,INT16,INT32,INT64,UINT8,UINT16,UINT32,UINT64,FLOAT,DOUBLE,BOOL,BIT,CSTRING"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"BYTE,INT8,INT16,INT32,INT64,UINT8,UINT16,UINT32,UINT64,FLOAT,DOUBLE,BOOL,BIT,STRING"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
fixed(tag): fixed cannot batch upload tags when value field is added to tag
</commit_message>
<xml_diff>
--- a/public/template/upload-tag-template.xlsx
+++ b/public/template/upload-tag-template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
   <si>
     <t>group</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>decimal</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
   <si>
     <t>groupName</t>
@@ -63,10 +66,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -85,14 +88,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -106,16 +102,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -130,68 +127,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,9 +162,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,6 +218,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,13 +240,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,13 +396,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,145 +414,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,6 +452,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -473,6 +491,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -484,32 +513,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,148 +536,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1004,15 +1007,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="23.2" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="23.2" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="15.0178571428571" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.4107142857143" style="1" customWidth="1"/>
@@ -1025,7 +1028,7 @@
     <col min="9" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1050,31 +1053,37 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(tag): template excel add new attributes and types
</commit_message>
<xml_diff>
--- a/public/template/upload-tag-template.xlsx
+++ b/public/template/upload-tag-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18120" windowHeight="12780"/>
+    <workbookView windowWidth="28060" windowHeight="15340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,8 +67,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -88,17 +88,47 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -110,9 +140,68 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,106 +215,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,181 +246,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,8 +437,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -447,31 +447,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,10 +469,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -513,6 +487,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,148 +536,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1012,7 +1012,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="23.2" outlineLevelRow="1"/>
@@ -1087,12 +1087,18 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 E1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5 D6:D7 D8:D13 D14:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+      <formula1>"Read,Write,Subscribe,Read Write,Read Subscribe,Write Subscribe,Read Write Subscribe,Static,Read Static,Write Static,Read Write Static,Subscribe Static, Read Subscribe Static, Write Subscribe Static,Read Write Subscribe Static"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+      <formula1>"BYTE,INT8,INT16,INT32,INT64,UINT8,UINT16,UINT32,UINT64,FLOAT,DOUBLE,BOOL,BIT,STRING,WORD,DWORD,LWORD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D5 D6:D7 D8:D13 D14:D1048576">
       <formula1>"Read,Write,Subscribe,Read Write,Read Subscribe,Write Subscribe,Read Write Subscribe"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576">
       <formula1>"BYTE,INT8,INT16,INT32,INT64,UINT8,UINT16,UINT32,UINT64,FLOAT,DOUBLE,BOOL,BIT,STRING"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
refactor(tag): Adjust column order in the template table
</commit_message>
<xml_diff>
--- a/public/template/upload-tag-template.xlsx
+++ b/public/template/upload-tag-template.xlsx
@@ -34,10 +34,10 @@
     <t>description</t>
   </si>
   <si>
+    <t>decimal</t>
+  </si>
+  <si>
     <t>precision</t>
-  </si>
-  <si>
-    <t>decimal</t>
   </si>
   <si>
     <t>value</t>
@@ -67,9 +67,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -101,6 +101,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -110,23 +118,98 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -140,92 +223,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,181 +246,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,25 +453,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,26 +484,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,147 +505,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1012,7 +1012,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="23.2" outlineLevelRow="1"/>
@@ -1023,8 +1023,8 @@
     <col min="4" max="4" width="30.8035714285714" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.1785714285714" style="1" customWidth="1"/>
     <col min="6" max="6" width="34.3660714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2589285714286" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.2589285714286" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>

</xml_diff>